<commit_message>
add empty merging func
</commit_message>
<xml_diff>
--- a/KB-25004 INV PLK CT DAP(1)_processed_text_rows.xlsx
+++ b/KB-25004 INV PLK CT DAP(1)_processed_text_rows.xlsx
@@ -2240,7 +2240,7 @@
       <c r="I13" s="133" t="n"/>
       <c r="J13" s="134" t="n"/>
     </row>
-    <row r="14" ht="23.1" customHeight="1" s="122">
+    <row r="14" ht="115.5" customHeight="1" s="122">
       <c r="A14" s="145" t="n"/>
       <c r="B14" s="146" t="n"/>
       <c r="C14" s="146" t="n"/>
@@ -2439,7 +2439,7 @@
     <row r="199"/>
     <row r="200" ht="23.1" customHeight="1" s="122"/>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="34">
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="F16:J16"/>
     <mergeCell ref="G1:J1"/>
@@ -2461,11 +2461,13 @@
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A14:E14"/>
     <mergeCell ref="F13:J13"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F14:J14"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A7:C7"/>

</xml_diff>